<commit_message>
Membership details test template committed
</commit_message>
<xml_diff>
--- a/test_data/orange_data.xlsx
+++ b/test_data/orange_data.xlsx
@@ -5,6 +5,7 @@
   <sheets>
     <sheet state="visible" name="Sheet1" sheetId="1" r:id="rId4"/>
     <sheet state="visible" name="Sheet2" sheetId="2" r:id="rId5"/>
+    <sheet state="visible" name="membership" sheetId="3" r:id="rId6"/>
   </sheets>
   <definedNames/>
   <calcPr/>
@@ -12,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="22">
   <si>
     <t>${username}</t>
   </si>
@@ -60,6 +61,24 @@
   </si>
   <si>
     <t>32</t>
+  </si>
+  <si>
+    <t>${membership}</t>
+  </si>
+  <si>
+    <t>${amount}</t>
+  </si>
+  <si>
+    <t>${currency}</t>
+  </si>
+  <si>
+    <t>ACCA</t>
+  </si>
+  <si>
+    <t>500</t>
+  </si>
+  <si>
+    <t>Indian Rupee</t>
   </si>
 </sst>
 </file>
@@ -96,7 +115,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -105,6 +124,9 @@
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="49" xfId="0" applyFont="1" applyNumberFormat="1"/>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="49" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+      <alignment readingOrder="0"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle xfId="0" name="Normal" builtinId="0"/>
@@ -118,6 +140,10 @@
 </file>
 
 <file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
 </file>
 
@@ -490,4 +516,116 @@
   </sheetData>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="0" summaryRight="0"/>
+  </sheetPr>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="D3" s="2"/>
+    </row>
+    <row r="4">
+      <c r="D4" s="2"/>
+    </row>
+    <row r="5">
+      <c r="D5" s="2"/>
+    </row>
+    <row r="6">
+      <c r="D6" s="2"/>
+    </row>
+    <row r="7">
+      <c r="D7" s="2"/>
+    </row>
+    <row r="8">
+      <c r="D8" s="2"/>
+    </row>
+    <row r="9">
+      <c r="D9" s="2"/>
+    </row>
+    <row r="10">
+      <c r="D10" s="2"/>
+    </row>
+    <row r="11">
+      <c r="D11" s="2"/>
+    </row>
+    <row r="12">
+      <c r="D12" s="2"/>
+    </row>
+    <row r="13">
+      <c r="D13" s="2"/>
+    </row>
+    <row r="14">
+      <c r="D14" s="2"/>
+    </row>
+    <row r="15">
+      <c r="D15" s="2"/>
+    </row>
+    <row r="16">
+      <c r="D16" s="2"/>
+    </row>
+    <row r="17">
+      <c r="D17" s="2"/>
+    </row>
+    <row r="18">
+      <c r="D18" s="2"/>
+    </row>
+    <row r="19">
+      <c r="D19" s="2"/>
+    </row>
+    <row r="20">
+      <c r="D20" s="2"/>
+    </row>
+    <row r="21">
+      <c r="D21" s="2"/>
+    </row>
+    <row r="22">
+      <c r="D22" s="2"/>
+    </row>
+    <row r="23">
+      <c r="D23" s="2"/>
+    </row>
+  </sheetData>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>